<commit_message>
Finalize study factors and properties term mapping
</commit_message>
<xml_diff>
--- a/doc/mapping results/termsMapping_studyFactorClassification.xlsx
+++ b/doc/mapping results/termsMapping_studyFactorClassification.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="5985" windowWidth="25170" windowHeight="6090" tabRatio="690"/>
+    <workbookView xWindow="30" yWindow="5985" windowWidth="25170" windowHeight="6090" tabRatio="884"/>
   </bookViews>
   <sheets>
     <sheet name="Summary StudyPropertyFactor" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="415">
   <si>
     <t>Foxa2</t>
   </si>
@@ -1048,24 +1048,12 @@
     <t>islet expansion in vitro</t>
   </si>
   <si>
-    <t>stress and apoptosis in islets or beta cells</t>
-  </si>
-  <si>
     <t>pancreas development</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/GO_0031016</t>
   </si>
   <si>
-    <t>new term in BCGO: 'response to stress' or apoptosis</t>
-  </si>
-  <si>
-    <t>new term in BCGO: exocrine or endocrine cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Or use CL:secretory cell, A cell that specializes in controlled release of one or more substances. </t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BCGO_0000083</t>
   </si>
   <si>
@@ -1081,16 +1069,6 @@
     <t>http://purl.obolibrary.org/obo/BCGO_0000087</t>
   </si>
   <si>
-    <t>Study is in the category of tissue expression, surveys and comparisons and specifically compares different types of cells in the endocrine and/or exocrine pancreas.</t>
-  </si>
-  <si>
-    <t>Study is in the category of Islet/beta-cell stimulation/injury and addresses stress sometimes as a means to induce apotosis in islets/ beta cells.</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Questions</t>
-  </si>
-  <si>
     <t>Experimental Factors</t>
   </si>
   <si>
@@ -1341,6 +1319,15 @@
   </si>
   <si>
     <t>Tissue</t>
+  </si>
+  <si>
+    <t>response to stress or apoptosis</t>
+  </si>
+  <si>
+    <t>secretory cell</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CL_0000151</t>
   </si>
 </sst>
 </file>
@@ -1887,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2441,10 +2428,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C54" s="22" t="s">
         <v>23</v>
@@ -2452,7 +2439,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>252</v>
@@ -2463,7 +2450,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>320</v>
@@ -2474,7 +2461,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>30</v>
@@ -2485,7 +2472,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>215</v>
@@ -2496,18 +2483,29 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>321</v>
+        <v>412</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>414</v>
+      </c>
+      <c r="B60" t="s">
+        <v>413</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="62" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="35" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2523,426 +2521,361 @@
     </row>
     <row r="64" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="B64" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C64" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="35" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A69" s="35" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>330</v>
+      </c>
+      <c r="B71" t="s">
+        <v>331</v>
+      </c>
+      <c r="C71" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>333</v>
+      </c>
+      <c r="B72" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B68" s="4" t="s">
+      <c r="C72" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>137</v>
-      </c>
-      <c r="B70" t="s">
-        <v>136</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>179</v>
+      <c r="A73" t="s">
+        <v>337</v>
+      </c>
+      <c r="B73" t="s">
+        <v>338</v>
       </c>
       <c r="C73" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
+      <c r="A74" t="s">
+        <v>340</v>
+      </c>
+      <c r="B74" t="s">
+        <v>341</v>
+      </c>
+      <c r="C74" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
+      <c r="A75" t="s">
+        <v>377</v>
+      </c>
+      <c r="B75" t="s">
+        <v>378</v>
+      </c>
+      <c r="C75" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-    </row>
-    <row r="77" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="35" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C78" s="11" t="s">
+      <c r="A76" t="s">
+        <v>346</v>
+      </c>
+      <c r="B76" t="s">
+        <v>347</v>
+      </c>
+      <c r="C76" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>344</v>
+      </c>
+      <c r="B77" t="s">
+        <v>345</v>
+      </c>
+      <c r="C77" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>349</v>
+      </c>
+      <c r="B78" t="s">
+        <v>350</v>
+      </c>
+      <c r="C78" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="B79" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="C79" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="B80" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="C80" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B81" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C81" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="B82" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C82" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>384</v>
+        <v>362</v>
       </c>
       <c r="B83" t="s">
-        <v>385</v>
+        <v>363</v>
       </c>
       <c r="C83" t="s">
-        <v>386</v>
+        <v>361</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B84" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="C84" t="s">
-        <v>349</v>
+        <v>364</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="B85" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
       <c r="C85" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>356</v>
+        <v>369</v>
       </c>
       <c r="B86" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="C86" t="s">
-        <v>355</v>
+        <v>368</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="B87" t="s">
-        <v>360</v>
+        <v>373</v>
       </c>
       <c r="C87" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>362</v>
+        <v>375</v>
       </c>
       <c r="B88" t="s">
-        <v>363</v>
+        <v>376</v>
       </c>
       <c r="C88" t="s">
-        <v>361</v>
+        <v>374</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="B89" t="s">
-        <v>348</v>
+        <v>382</v>
       </c>
       <c r="C89" t="s">
-        <v>364</v>
+        <v>380</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>366</v>
+        <v>383</v>
       </c>
       <c r="B90" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
       <c r="C90" t="s">
-        <v>365</v>
+        <v>380</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>369</v>
+        <v>385</v>
       </c>
       <c r="B91" t="s">
-        <v>370</v>
+        <v>386</v>
       </c>
       <c r="C91" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>347</v>
+        <v>387</v>
       </c>
       <c r="B92" t="s">
-        <v>348</v>
+        <v>388</v>
       </c>
       <c r="C92" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>373</v>
+        <v>389</v>
       </c>
       <c r="B93" t="s">
-        <v>374</v>
+        <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>372</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>376</v>
+        <v>391</v>
       </c>
       <c r="B94" t="s">
-        <v>377</v>
+        <v>392</v>
       </c>
       <c r="C94" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>379</v>
+        <v>394</v>
       </c>
       <c r="B95" t="s">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="C95" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>382</v>
+        <v>397</v>
       </c>
       <c r="B96" t="s">
-        <v>383</v>
+        <v>398</v>
       </c>
       <c r="C96" t="s">
-        <v>381</v>
+        <v>396</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
       <c r="B97" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="C97" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="B98" t="s">
-        <v>391</v>
+        <v>404</v>
       </c>
       <c r="C98" t="s">
-        <v>387</v>
+        <v>402</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
       <c r="B99" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="C99" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>394</v>
-      </c>
-      <c r="B100" t="s">
-        <v>395</v>
-      </c>
-      <c r="C100" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>396</v>
-      </c>
-      <c r="B101" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>398</v>
-      </c>
-      <c r="B102" t="s">
-        <v>399</v>
-      </c>
-      <c r="C102" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>401</v>
-      </c>
-      <c r="B103" t="s">
-        <v>402</v>
-      </c>
-      <c r="C103" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>404</v>
-      </c>
-      <c r="B104" t="s">
         <v>405</v>
-      </c>
-      <c r="C104" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>407</v>
-      </c>
-      <c r="B105" t="s">
-        <v>408</v>
-      </c>
-      <c r="C105" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>410</v>
-      </c>
-      <c r="B106" t="s">
-        <v>411</v>
-      </c>
-      <c r="C106" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>413</v>
-      </c>
-      <c r="B107" t="s">
-        <v>414</v>
-      </c>
-      <c r="C107" t="s">
-        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -3640,7 +3573,7 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -4804,7 +4737,7 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>